<commit_message>
Updated graphs and dependent data sources
</commit_message>
<xml_diff>
--- a/docs/performance.xlsx
+++ b/docs/performance.xlsx
@@ -5,20 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22e8633286bd19a7/Documents/dev/map-reduce/docs/intel/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22e8633286bd19a7/Documents/dev/map-reduce/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="232" documentId="8_{8E589E63-48AD-4E69-8076-DD012BDE5EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{73203EA1-32F6-4706-8ECD-1D6AF7AEA69C}"/>
+  <xr:revisionPtr revIDLastSave="241" documentId="8_{8E589E63-48AD-4E69-8076-DD012BDE5EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A335181C-6024-4FB4-BCDA-B3B864BF376D}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" xr2:uid="{9DF68624-D4B9-4083-BFAE-DE2CA7971FFA}"/>
+    <workbookView xWindow="28702" yWindow="-98" windowWidth="28995" windowHeight="15675" activeTab="1" xr2:uid="{9DF68624-D4B9-4083-BFAE-DE2CA7971FFA}"/>
   </bookViews>
   <sheets>
     <sheet name="Intel CPU" sheetId="1" r:id="rId1"/>
     <sheet name="AMD CPU" sheetId="2" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -2543,28 +2540,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.5299999999999998E-2</c:v>
+                  <c:v>1.2499999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.38E-2</c:v>
+                  <c:v>1.5599999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.13320000000000001</c:v>
+                  <c:v>0.1051</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.5338000000000001</c:v>
+                  <c:v>1.5004999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>13.767399999999999</c:v>
+                  <c:v>13.267099999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>118.60570000000001</c:v>
+                  <c:v>108.9691</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1022.258</c:v>
+                  <c:v>1141.125</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>10462.210000000001</c:v>
+                  <c:v>10842.32</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2660,28 +2657,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.96619999999999995</c:v>
+                  <c:v>0.86330000000000007</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.0487</c:v>
+                  <c:v>0.98099999999999998</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3159999999999998</c:v>
+                  <c:v>1.2426999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.7806</c:v>
+                  <c:v>1.7097999999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.6591999999999993</c:v>
+                  <c:v>5.8231999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>35.364199999999997</c:v>
+                  <c:v>31.437899999999999</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>298.73950000000002</c:v>
+                  <c:v>290.43439999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2982.2883000000002</c:v>
+                  <c:v>2898.2640000000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2771,28 +2768,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.3261E-2</c:v>
+                  <c:v>1.2020999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.1809999999999999E-3</c:v>
+                  <c:v>9.0799999999999995E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.8535000000000008E-2</c:v>
+                  <c:v>7.8493000000000007E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.75371299999999997</c:v>
+                  <c:v>0.79042699999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.7903689999999992</c:v>
+                  <c:v>8.5193000000000012</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>66.46069</c:v>
+                  <c:v>90.207599999999985</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>660.08050000000003</c:v>
+                  <c:v>828.64599999999996</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9478.5969999999998</c:v>
+                  <c:v>8313.6299999999992</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2882,28 +2879,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.6995840000000002</c:v>
+                  <c:v>1.3681949999999998</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1212899999999999</c:v>
+                  <c:v>1.6355469999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.424477</c:v>
+                  <c:v>1.7081529999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4679379999999997</c:v>
+                  <c:v>2.0617509999999997</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.5098760000000002</c:v>
+                  <c:v>4.7829629999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>18.800899999999999</c:v>
+                  <c:v>29.55997</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>142.20162999999999</c:v>
+                  <c:v>252.88990000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1331.6327999999999</c:v>
+                  <c:v>2272.384</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3407,28 +3404,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.4599999999999998E-2</c:v>
+                  <c:v>1.21E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.1299999999999999E-2</c:v>
+                  <c:v>1.3399999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.10490000000000001</c:v>
+                  <c:v>8.2699999999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2861</c:v>
+                  <c:v>1.2745</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.281599999999999</c:v>
+                  <c:v>11.135899999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>95.121000000000009</c:v>
+                  <c:v>85.954999999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>813.226</c:v>
+                  <c:v>896.14199999999994</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>8356.2000000000007</c:v>
+                  <c:v>8565.61</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3524,28 +3521,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.89380000000000004</c:v>
+                  <c:v>0.81059999999999999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.99609999999999999</c:v>
+                  <c:v>0.9335</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.2238</c:v>
+                  <c:v>1.1709999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.4469999999999998</c:v>
+                  <c:v>1.4058999999999999</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.1673999999999998</c:v>
+                  <c:v>1.8571</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.5765000000000002</c:v>
+                  <c:v>6.0327000000000002</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.401800000000001</c:v>
+                  <c:v>35.4497</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>268.22629999999998</c:v>
+                  <c:v>300.29699999999997</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3635,28 +3632,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.3178E-2</c:v>
+                  <c:v>1.1790999999999999E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.7489999999999998E-3</c:v>
+                  <c:v>7.6150000000000002E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.4660000000000004E-2</c:v>
+                  <c:v>6.4229000000000008E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.717862</c:v>
+                  <c:v>0.64806600000000003</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.4469899999999996</c:v>
+                  <c:v>7.1145200000000006</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>63.239999999999995</c:v>
+                  <c:v>73.675299999999993</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>626.78700000000003</c:v>
+                  <c:v>692.91399999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9150.2099999999991</c:v>
+                  <c:v>6861.78</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3746,28 +3743,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>1.6184690000000002</c:v>
+                  <c:v>1.274235</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.036511</c:v>
+                  <c:v>1.5183119999999999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1.3197239999999999</c:v>
+                  <c:v>1.5844999999999998</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.2970569999999999</c:v>
+                  <c:v>1.7759519999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.3543050000000001</c:v>
+                  <c:v>2.51614</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.0670299999999999</c:v>
+                  <c:v>8.739980000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>30.019930000000002</c:v>
+                  <c:v>37.228900000000003</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>252.33579999999998</c:v>
+                  <c:v>320.26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6854,281 +6851,6 @@
 </c:userShapes>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <xxl21:alternateUrls>
-      <xxl21:absoluteUrl r:id="rId2"/>
-    </xxl21:alternateUrls>
-    <sheetNames>
-      <sheetName val="AMD CPU"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0">
-        <row r="1">
-          <cell r="E1" t="str">
-            <v>MSVC (WIN11) Core (ms)</v>
-          </cell>
-          <cell r="F1" t="str">
-            <v>MSVC (WIN11) Total (ms)</v>
-          </cell>
-          <cell r="K1" t="str">
-            <v>NVCC (WIN11) Core (ms)</v>
-          </cell>
-          <cell r="L1" t="str">
-            <v>NVCC (WIN11) Total (ms)</v>
-          </cell>
-          <cell r="P1" t="str">
-            <v>GCC (WSL2) Core (ms)</v>
-          </cell>
-          <cell r="Q1" t="str">
-            <v>GCC (WSL2) Total (ms)</v>
-          </cell>
-          <cell r="V1" t="str">
-            <v>NVCC (WSL2) Core (ms)</v>
-          </cell>
-          <cell r="W1" t="str">
-            <v>NVCC (WSL2) Total (ms)</v>
-          </cell>
-        </row>
-        <row r="2">
-          <cell r="A2">
-            <v>10</v>
-          </cell>
-          <cell r="E2">
-            <v>1.4599999999999998E-2</v>
-          </cell>
-          <cell r="F2">
-            <v>1.5299999999999998E-2</v>
-          </cell>
-          <cell r="K2">
-            <v>0.89380000000000004</v>
-          </cell>
-          <cell r="L2">
-            <v>0.96619999999999995</v>
-          </cell>
-          <cell r="P2">
-            <v>1.3178E-2</v>
-          </cell>
-          <cell r="Q2">
-            <v>1.3261E-2</v>
-          </cell>
-          <cell r="V2">
-            <v>1.6184690000000002</v>
-          </cell>
-          <cell r="W2">
-            <v>1.6995840000000002</v>
-          </cell>
-        </row>
-        <row r="3">
-          <cell r="A3">
-            <v>100</v>
-          </cell>
-          <cell r="E3">
-            <v>1.1299999999999999E-2</v>
-          </cell>
-          <cell r="F3">
-            <v>1.38E-2</v>
-          </cell>
-          <cell r="K3">
-            <v>0.99609999999999999</v>
-          </cell>
-          <cell r="L3">
-            <v>1.0487</v>
-          </cell>
-          <cell r="P3">
-            <v>6.7489999999999998E-3</v>
-          </cell>
-          <cell r="Q3">
-            <v>7.1809999999999999E-3</v>
-          </cell>
-          <cell r="V3">
-            <v>1.036511</v>
-          </cell>
-          <cell r="W3">
-            <v>1.1212899999999999</v>
-          </cell>
-        </row>
-        <row r="4">
-          <cell r="A4">
-            <v>1000</v>
-          </cell>
-          <cell r="E4">
-            <v>0.10490000000000001</v>
-          </cell>
-          <cell r="F4">
-            <v>0.13320000000000001</v>
-          </cell>
-          <cell r="K4">
-            <v>1.2238</v>
-          </cell>
-          <cell r="L4">
-            <v>1.3159999999999998</v>
-          </cell>
-          <cell r="P4">
-            <v>7.4660000000000004E-2</v>
-          </cell>
-          <cell r="Q4">
-            <v>7.8535000000000008E-2</v>
-          </cell>
-          <cell r="V4">
-            <v>1.3197239999999999</v>
-          </cell>
-          <cell r="W4">
-            <v>1.424477</v>
-          </cell>
-        </row>
-        <row r="5">
-          <cell r="A5">
-            <v>10000</v>
-          </cell>
-          <cell r="E5">
-            <v>1.2861</v>
-          </cell>
-          <cell r="F5">
-            <v>1.5338000000000001</v>
-          </cell>
-          <cell r="K5">
-            <v>1.4469999999999998</v>
-          </cell>
-          <cell r="L5">
-            <v>1.7806</v>
-          </cell>
-          <cell r="P5">
-            <v>0.717862</v>
-          </cell>
-          <cell r="Q5">
-            <v>0.75371299999999997</v>
-          </cell>
-          <cell r="V5">
-            <v>1.2970569999999999</v>
-          </cell>
-          <cell r="W5">
-            <v>1.4679379999999997</v>
-          </cell>
-        </row>
-        <row r="6">
-          <cell r="A6">
-            <v>100000</v>
-          </cell>
-          <cell r="E6">
-            <v>11.281599999999999</v>
-          </cell>
-          <cell r="F6">
-            <v>13.767399999999999</v>
-          </cell>
-          <cell r="K6">
-            <v>3.1673999999999998</v>
-          </cell>
-          <cell r="L6">
-            <v>7.6591999999999993</v>
-          </cell>
-          <cell r="P6">
-            <v>7.4469899999999996</v>
-          </cell>
-          <cell r="Q6">
-            <v>7.7903689999999992</v>
-          </cell>
-          <cell r="V6">
-            <v>3.3543050000000001</v>
-          </cell>
-          <cell r="W6">
-            <v>4.5098760000000002</v>
-          </cell>
-        </row>
-        <row r="7">
-          <cell r="A7">
-            <v>1000000</v>
-          </cell>
-          <cell r="E7">
-            <v>95.121000000000009</v>
-          </cell>
-          <cell r="F7">
-            <v>118.60570000000001</v>
-          </cell>
-          <cell r="K7">
-            <v>5.5765000000000002</v>
-          </cell>
-          <cell r="L7">
-            <v>35.364199999999997</v>
-          </cell>
-          <cell r="P7">
-            <v>63.239999999999995</v>
-          </cell>
-          <cell r="Q7">
-            <v>66.46069</v>
-          </cell>
-          <cell r="V7">
-            <v>7.0670299999999999</v>
-          </cell>
-          <cell r="W7">
-            <v>18.800899999999999</v>
-          </cell>
-        </row>
-        <row r="8">
-          <cell r="A8">
-            <v>10000000</v>
-          </cell>
-          <cell r="E8">
-            <v>813.226</v>
-          </cell>
-          <cell r="F8">
-            <v>1022.258</v>
-          </cell>
-          <cell r="K8">
-            <v>30.401800000000001</v>
-          </cell>
-          <cell r="L8">
-            <v>298.73950000000002</v>
-          </cell>
-          <cell r="P8">
-            <v>626.78700000000003</v>
-          </cell>
-          <cell r="Q8">
-            <v>660.08050000000003</v>
-          </cell>
-          <cell r="V8">
-            <v>30.019930000000002</v>
-          </cell>
-          <cell r="W8">
-            <v>142.20162999999999</v>
-          </cell>
-        </row>
-        <row r="9">
-          <cell r="A9">
-            <v>100000000</v>
-          </cell>
-          <cell r="E9">
-            <v>8356.2000000000007</v>
-          </cell>
-          <cell r="F9">
-            <v>10462.210000000001</v>
-          </cell>
-          <cell r="K9">
-            <v>268.22629999999998</v>
-          </cell>
-          <cell r="L9">
-            <v>2982.2883000000002</v>
-          </cell>
-          <cell r="P9">
-            <v>9150.2099999999991</v>
-          </cell>
-          <cell r="Q9">
-            <v>9478.5969999999998</v>
-          </cell>
-          <cell r="V9">
-            <v>252.33579999999998</v>
-          </cell>
-          <cell r="W9">
-            <v>1331.6327999999999</v>
-          </cell>
-        </row>
-      </sheetData>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
-</file>
-
 <file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
 <personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
@@ -7452,750 +7174,6 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE75E16D-024E-4063-A895-F36D0968513C}">
   <dimension ref="A1:W9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C28" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
-  <cols>
-    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.53125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.53125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.19921875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.9296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.19921875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.19921875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.53125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.19921875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.9296875" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" t="s">
-        <v>18</v>
-      </c>
-      <c r="T1" t="s">
-        <v>19</v>
-      </c>
-      <c r="U1" t="s">
-        <v>20</v>
-      </c>
-      <c r="V1" t="s">
-        <v>21</v>
-      </c>
-      <c r="W1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A2" s="1">
-        <v>10</v>
-      </c>
-      <c r="B2">
-        <v>3.3999999999999998E-3</v>
-      </c>
-      <c r="C2">
-        <v>1.1000000000000001E-3</v>
-      </c>
-      <c r="D2">
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="E2">
-        <f>SUM(B2:C2)</f>
-        <v>4.4999999999999997E-3</v>
-      </c>
-      <c r="F2">
-        <f>SUM(B2:D2)</f>
-        <v>4.7999999999999996E-3</v>
-      </c>
-      <c r="G2">
-        <v>8.7499999999999994E-2</v>
-      </c>
-      <c r="H2">
-        <v>0.25969999999999999</v>
-      </c>
-      <c r="I2">
-        <v>6.1400000000000003E-2</v>
-      </c>
-      <c r="J2">
-        <v>8.5000000000000006E-3</v>
-      </c>
-      <c r="K2">
-        <f>SUM(G2:H2)</f>
-        <v>0.34719999999999995</v>
-      </c>
-      <c r="L2">
-        <f t="shared" ref="L2:L9" si="0">SUM(G2:J2)</f>
-        <v>0.41709999999999997</v>
-      </c>
-      <c r="M2">
-        <v>6.718E-3</v>
-      </c>
-      <c r="N2">
-        <v>1.008E-3</v>
-      </c>
-      <c r="O2" s="2">
-        <v>8.3999999999999995E-5</v>
-      </c>
-      <c r="P2">
-        <f>SUM(M2:N2)</f>
-        <v>7.7260000000000002E-3</v>
-      </c>
-      <c r="Q2">
-        <f t="shared" ref="Q2:Q9" si="1">SUM(M2:O2)</f>
-        <v>7.8100000000000001E-3</v>
-      </c>
-      <c r="R2">
-        <v>0.20544100000000001</v>
-      </c>
-      <c r="S2">
-        <v>0.190054</v>
-      </c>
-      <c r="T2">
-        <v>6.2382E-2</v>
-      </c>
-      <c r="U2">
-        <v>1.4100000000000001E-4</v>
-      </c>
-      <c r="V2">
-        <f>SUM(R2:S2)</f>
-        <v>0.39549500000000004</v>
-      </c>
-      <c r="W2">
-        <f t="shared" ref="W2:W9" si="2">SUM(R2:U2)</f>
-        <v>0.45801800000000004</v>
-      </c>
-    </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A3" s="1">
-        <v>100</v>
-      </c>
-      <c r="B3">
-        <v>5.4999999999999997E-3</v>
-      </c>
-      <c r="C3">
-        <v>1.6999999999999999E-3</v>
-      </c>
-      <c r="D3">
-        <v>1.4E-3</v>
-      </c>
-      <c r="E3">
-        <f t="shared" ref="E3:E9" si="3">SUM(B3:C3)</f>
-        <v>7.1999999999999998E-3</v>
-      </c>
-      <c r="F3">
-        <f t="shared" ref="F3:F9" si="4">SUM(B3:D3)</f>
-        <v>8.6E-3</v>
-      </c>
-      <c r="G3">
-        <v>8.5400000000000004E-2</v>
-      </c>
-      <c r="H3">
-        <v>0.3075</v>
-      </c>
-      <c r="I3">
-        <v>5.28E-2</v>
-      </c>
-      <c r="J3">
-        <v>1.5E-3</v>
-      </c>
-      <c r="K3">
-        <f t="shared" ref="K3:K9" si="5">SUM(G3:H3)</f>
-        <v>0.39290000000000003</v>
-      </c>
-      <c r="L3">
-        <f t="shared" si="0"/>
-        <v>0.44720000000000004</v>
-      </c>
-      <c r="M3">
-        <v>3.4970000000000001E-3</v>
-      </c>
-      <c r="N3">
-        <v>1.0859999999999999E-3</v>
-      </c>
-      <c r="O3">
-        <v>2.6600000000000001E-4</v>
-      </c>
-      <c r="P3">
-        <f t="shared" ref="P3:P9" si="6">SUM(M3:N3)</f>
-        <v>4.5830000000000003E-3</v>
-      </c>
-      <c r="Q3">
-        <f t="shared" si="1"/>
-        <v>4.849E-3</v>
-      </c>
-      <c r="R3">
-        <v>0.19217400000000001</v>
-      </c>
-      <c r="S3">
-        <v>0.21096799999999999</v>
-      </c>
-      <c r="T3">
-        <v>6.3317999999999999E-2</v>
-      </c>
-      <c r="U3">
-        <v>5.8299999999999997E-4</v>
-      </c>
-      <c r="V3">
-        <f t="shared" ref="V3:V9" si="7">SUM(R3:S3)</f>
-        <v>0.403142</v>
-      </c>
-      <c r="W3">
-        <f t="shared" si="2"/>
-        <v>0.46704299999999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A4" s="1">
-        <v>1000</v>
-      </c>
-      <c r="B4">
-        <v>4.6100000000000002E-2</v>
-      </c>
-      <c r="C4">
-        <v>1.26E-2</v>
-      </c>
-      <c r="D4">
-        <v>1.34E-2</v>
-      </c>
-      <c r="E4">
-        <f t="shared" si="3"/>
-        <v>5.8700000000000002E-2</v>
-      </c>
-      <c r="F4">
-        <f t="shared" si="4"/>
-        <v>7.2099999999999997E-2</v>
-      </c>
-      <c r="G4">
-        <v>5.9400000000000001E-2</v>
-      </c>
-      <c r="H4">
-        <v>0.31919999999999998</v>
-      </c>
-      <c r="I4">
-        <v>6.1199999999999997E-2</v>
-      </c>
-      <c r="J4">
-        <v>1.3599999999999999E-2</v>
-      </c>
-      <c r="K4">
-        <f t="shared" si="5"/>
-        <v>0.37859999999999999</v>
-      </c>
-      <c r="L4">
-        <f t="shared" si="0"/>
-        <v>0.45339999999999997</v>
-      </c>
-      <c r="M4">
-        <v>3.4388000000000002E-2</v>
-      </c>
-      <c r="N4">
-        <v>1.1872000000000001E-2</v>
-      </c>
-      <c r="O4">
-        <v>2.2729999999999998E-3</v>
-      </c>
-      <c r="P4">
-        <f t="shared" si="6"/>
-        <v>4.6260000000000003E-2</v>
-      </c>
-      <c r="Q4">
-        <f t="shared" si="1"/>
-        <v>4.8533E-2</v>
-      </c>
-      <c r="R4">
-        <v>0.186225</v>
-      </c>
-      <c r="S4">
-        <v>0.24310399999999999</v>
-      </c>
-      <c r="T4">
-        <v>6.6530000000000006E-2</v>
-      </c>
-      <c r="U4">
-        <v>4.7790000000000003E-3</v>
-      </c>
-      <c r="V4">
-        <f t="shared" si="7"/>
-        <v>0.42932899999999996</v>
-      </c>
-      <c r="W4">
-        <f t="shared" si="2"/>
-        <v>0.50063799999999992</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A5" s="1">
-        <v>10000</v>
-      </c>
-      <c r="B5">
-        <v>0.43590000000000001</v>
-      </c>
-      <c r="C5">
-        <v>0.1149</v>
-      </c>
-      <c r="D5">
-        <v>0.13370000000000001</v>
-      </c>
-      <c r="E5">
-        <f t="shared" si="3"/>
-        <v>0.55079999999999996</v>
-      </c>
-      <c r="F5">
-        <f t="shared" si="4"/>
-        <v>0.6845</v>
-      </c>
-      <c r="G5">
-        <v>5.79E-2</v>
-      </c>
-      <c r="H5">
-        <v>0.3659</v>
-      </c>
-      <c r="I5">
-        <v>9.6100000000000005E-2</v>
-      </c>
-      <c r="J5">
-        <v>0.1338</v>
-      </c>
-      <c r="K5">
-        <f t="shared" si="5"/>
-        <v>0.42380000000000001</v>
-      </c>
-      <c r="L5">
-        <f t="shared" si="0"/>
-        <v>0.65370000000000006</v>
-      </c>
-      <c r="M5">
-        <v>0.331374</v>
-      </c>
-      <c r="N5">
-        <v>0.12942100000000001</v>
-      </c>
-      <c r="O5">
-        <v>2.4208E-2</v>
-      </c>
-      <c r="P5">
-        <f t="shared" si="6"/>
-        <v>0.46079500000000001</v>
-      </c>
-      <c r="Q5">
-        <f t="shared" si="1"/>
-        <v>0.48500300000000002</v>
-      </c>
-      <c r="R5">
-        <v>0.203847</v>
-      </c>
-      <c r="S5">
-        <v>0.29677300000000001</v>
-      </c>
-      <c r="T5">
-        <v>8.2985000000000003E-2</v>
-      </c>
-      <c r="U5">
-        <v>5.4524999999999997E-2</v>
-      </c>
-      <c r="V5">
-        <f t="shared" si="7"/>
-        <v>0.50062000000000006</v>
-      </c>
-      <c r="W5">
-        <f t="shared" si="2"/>
-        <v>0.63813000000000009</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A6" s="1">
-        <v>100000</v>
-      </c>
-      <c r="B6">
-        <v>4.6462000000000003</v>
-      </c>
-      <c r="C6">
-        <v>1.2143999999999999</v>
-      </c>
-      <c r="D6">
-        <v>1.4245000000000001</v>
-      </c>
-      <c r="E6">
-        <f t="shared" si="3"/>
-        <v>5.8605999999999998</v>
-      </c>
-      <c r="F6">
-        <f t="shared" si="4"/>
-        <v>7.2850999999999999</v>
-      </c>
-      <c r="G6">
-        <v>6.0600000000000001E-2</v>
-      </c>
-      <c r="H6">
-        <v>1.2386999999999999</v>
-      </c>
-      <c r="I6">
-        <v>0.51359999999999995</v>
-      </c>
-      <c r="J6">
-        <v>1.3708</v>
-      </c>
-      <c r="K6">
-        <f t="shared" si="5"/>
-        <v>1.2992999999999999</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="0"/>
-        <v>3.1837</v>
-      </c>
-      <c r="M6">
-        <v>3.3493400000000002</v>
-      </c>
-      <c r="N6">
-        <v>1.3481300000000001</v>
-      </c>
-      <c r="O6">
-        <v>0.23305300000000001</v>
-      </c>
-      <c r="P6">
-        <f t="shared" si="6"/>
-        <v>4.69747</v>
-      </c>
-      <c r="Q6">
-        <f t="shared" si="1"/>
-        <v>4.930523</v>
-      </c>
-      <c r="R6">
-        <v>0.18995100000000001</v>
-      </c>
-      <c r="S6">
-        <v>1.48854</v>
-      </c>
-      <c r="T6">
-        <v>0.31885000000000002</v>
-      </c>
-      <c r="U6">
-        <v>0.47934500000000002</v>
-      </c>
-      <c r="V6">
-        <f t="shared" si="7"/>
-        <v>1.678491</v>
-      </c>
-      <c r="W6">
-        <f t="shared" si="2"/>
-        <v>2.4766859999999999</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A7" s="1">
-        <v>1000000</v>
-      </c>
-      <c r="B7">
-        <v>41.9816</v>
-      </c>
-      <c r="C7">
-        <v>15.0382</v>
-      </c>
-      <c r="D7">
-        <v>12.792</v>
-      </c>
-      <c r="E7">
-        <f t="shared" si="3"/>
-        <v>57.019800000000004</v>
-      </c>
-      <c r="F7">
-        <f t="shared" si="4"/>
-        <v>69.811800000000005</v>
-      </c>
-      <c r="G7">
-        <v>0.17019999999999999</v>
-      </c>
-      <c r="H7">
-        <v>5.6425000000000001</v>
-      </c>
-      <c r="I7">
-        <v>4.1814999999999998</v>
-      </c>
-      <c r="J7">
-        <v>12.843299999999999</v>
-      </c>
-      <c r="K7">
-        <f t="shared" si="5"/>
-        <v>5.8127000000000004</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="0"/>
-        <v>22.837499999999999</v>
-      </c>
-      <c r="M7">
-        <v>31.771699999999999</v>
-      </c>
-      <c r="N7">
-        <v>15.199400000000001</v>
-      </c>
-      <c r="O7">
-        <v>2.6561699999999999</v>
-      </c>
-      <c r="P7">
-        <f t="shared" si="6"/>
-        <v>46.9711</v>
-      </c>
-      <c r="Q7">
-        <f t="shared" si="1"/>
-        <v>49.627270000000003</v>
-      </c>
-      <c r="R7">
-        <v>0.40144400000000002</v>
-      </c>
-      <c r="S7">
-        <v>5.6603300000000001</v>
-      </c>
-      <c r="T7">
-        <v>5.20688</v>
-      </c>
-      <c r="U7">
-        <v>4.4508200000000002</v>
-      </c>
-      <c r="V7">
-        <f t="shared" si="7"/>
-        <v>6.0617739999999998</v>
-      </c>
-      <c r="W7">
-        <f t="shared" si="2"/>
-        <v>15.719474</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A8" s="1">
-        <v>10000000</v>
-      </c>
-      <c r="B8">
-        <v>412.77499999999998</v>
-      </c>
-      <c r="C8">
-        <v>149.72</v>
-      </c>
-      <c r="D8">
-        <v>127.27500000000001</v>
-      </c>
-      <c r="E8">
-        <f t="shared" si="3"/>
-        <v>562.495</v>
-      </c>
-      <c r="F8">
-        <f t="shared" si="4"/>
-        <v>689.77</v>
-      </c>
-      <c r="G8">
-        <v>0.92459999999999998</v>
-      </c>
-      <c r="H8">
-        <v>44.822099999999999</v>
-      </c>
-      <c r="I8">
-        <v>39.967799999999997</v>
-      </c>
-      <c r="J8">
-        <v>127.074</v>
-      </c>
-      <c r="K8">
-        <f t="shared" si="5"/>
-        <v>45.746699999999997</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="0"/>
-        <v>212.7885</v>
-      </c>
-      <c r="M8">
-        <v>307.89400000000001</v>
-      </c>
-      <c r="N8">
-        <v>127.69</v>
-      </c>
-      <c r="O8">
-        <v>22.965199999999999</v>
-      </c>
-      <c r="P8">
-        <f t="shared" si="6"/>
-        <v>435.584</v>
-      </c>
-      <c r="Q8">
-        <f t="shared" si="1"/>
-        <v>458.54919999999998</v>
-      </c>
-      <c r="R8">
-        <v>1.5768500000000001</v>
-      </c>
-      <c r="S8">
-        <v>43.444499999999998</v>
-      </c>
-      <c r="T8">
-        <v>47.012700000000002</v>
-      </c>
-      <c r="U8">
-        <v>43.414999999999999</v>
-      </c>
-      <c r="V8">
-        <f t="shared" si="7"/>
-        <v>45.021349999999998</v>
-      </c>
-      <c r="W8">
-        <f t="shared" si="2"/>
-        <v>135.44905</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.45">
-      <c r="A9" s="1">
-        <v>100000000</v>
-      </c>
-      <c r="B9">
-        <v>4283.7299999999996</v>
-      </c>
-      <c r="C9">
-        <v>1427.25</v>
-      </c>
-      <c r="D9">
-        <v>1278.49</v>
-      </c>
-      <c r="E9">
-        <f t="shared" si="3"/>
-        <v>5710.98</v>
-      </c>
-      <c r="F9">
-        <f t="shared" si="4"/>
-        <v>6989.4699999999993</v>
-      </c>
-      <c r="G9">
-        <v>2.8048999999999999</v>
-      </c>
-      <c r="H9">
-        <v>405.38400000000001</v>
-      </c>
-      <c r="I9">
-        <v>400.85500000000002</v>
-      </c>
-      <c r="J9">
-        <v>1301.2</v>
-      </c>
-      <c r="K9">
-        <f t="shared" si="5"/>
-        <v>408.18889999999999</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="0"/>
-        <v>2110.2438999999999</v>
-      </c>
-      <c r="M9">
-        <v>3130.81</v>
-      </c>
-      <c r="N9">
-        <v>1366.69</v>
-      </c>
-      <c r="O9">
-        <v>248.45500000000001</v>
-      </c>
-      <c r="P9">
-        <f t="shared" si="6"/>
-        <v>4497.5</v>
-      </c>
-      <c r="Q9">
-        <f t="shared" si="1"/>
-        <v>4745.9549999999999</v>
-      </c>
-      <c r="R9">
-        <v>7.3137499999999998</v>
-      </c>
-      <c r="S9">
-        <v>408.22899999999998</v>
-      </c>
-      <c r="T9">
-        <v>547.71600000000001</v>
-      </c>
-      <c r="U9">
-        <v>449.26600000000002</v>
-      </c>
-      <c r="V9">
-        <f t="shared" si="7"/>
-        <v>415.54275000000001</v>
-      </c>
-      <c r="W9">
-        <f t="shared" si="2"/>
-        <v>1412.52475</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CF9CBA4-1D0E-4C7D-85A3-E5E8BE03303C}">
-  <dimension ref="A1:W9"/>
-  <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8301,78 +7279,78 @@
         <v>10</v>
       </c>
       <c r="B2">
-        <v>8.3999999999999995E-3</v>
+        <v>3.3999999999999998E-3</v>
       </c>
       <c r="C2">
-        <v>6.1999999999999998E-3</v>
+        <v>1.1000000000000001E-3</v>
       </c>
       <c r="D2">
-        <v>6.9999999999999999E-4</v>
+        <v>2.9999999999999997E-4</v>
       </c>
       <c r="E2">
         <f>SUM(B2:C2)</f>
-        <v>1.4599999999999998E-2</v>
+        <v>4.4999999999999997E-3</v>
       </c>
       <c r="F2">
         <f>SUM(B2:D2)</f>
-        <v>1.5299999999999998E-2</v>
+        <v>4.7999999999999996E-3</v>
       </c>
       <c r="G2">
-        <v>0.2147</v>
+        <v>8.7499999999999994E-2</v>
       </c>
       <c r="H2">
-        <v>0.67910000000000004</v>
+        <v>0.25969999999999999</v>
       </c>
       <c r="I2">
-        <v>7.1999999999999995E-2</v>
+        <v>6.1400000000000003E-2</v>
       </c>
       <c r="J2">
-        <v>4.0000000000000002E-4</v>
+        <v>8.5000000000000006E-3</v>
       </c>
       <c r="K2">
         <f>SUM(G2:H2)</f>
-        <v>0.89380000000000004</v>
+        <v>0.34719999999999995</v>
       </c>
       <c r="L2">
         <f t="shared" ref="L2:L9" si="0">SUM(G2:J2)</f>
-        <v>0.96619999999999995</v>
+        <v>0.41709999999999997</v>
       </c>
       <c r="M2">
-        <v>1.1736E-2</v>
+        <v>6.718E-3</v>
       </c>
       <c r="N2">
-        <v>1.4419999999999999E-3</v>
+        <v>1.008E-3</v>
       </c>
       <c r="O2" s="2">
-        <v>8.2999999999999998E-5</v>
+        <v>8.3999999999999995E-5</v>
       </c>
       <c r="P2">
         <f>SUM(M2:N2)</f>
-        <v>1.3178E-2</v>
+        <v>7.7260000000000002E-3</v>
       </c>
       <c r="Q2">
         <f t="shared" ref="Q2:Q9" si="1">SUM(M2:O2)</f>
-        <v>1.3261E-2</v>
+        <v>7.8100000000000001E-3</v>
       </c>
       <c r="R2">
-        <v>0.52131899999999998</v>
+        <v>0.20544100000000001</v>
       </c>
       <c r="S2">
-        <v>1.0971500000000001</v>
+        <v>0.190054</v>
       </c>
       <c r="T2">
-        <v>8.0784999999999996E-2</v>
+        <v>6.2382E-2</v>
       </c>
       <c r="U2">
-        <v>3.3E-4</v>
+        <v>1.4100000000000001E-4</v>
       </c>
       <c r="V2">
         <f>SUM(R2:S2)</f>
-        <v>1.6184690000000002</v>
+        <v>0.39549500000000004</v>
       </c>
       <c r="W2">
         <f t="shared" ref="W2:W9" si="2">SUM(R2:U2)</f>
-        <v>1.6995840000000002</v>
+        <v>0.45801800000000004</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.45">
@@ -8380,78 +7358,78 @@
         <v>100</v>
       </c>
       <c r="B3">
-        <v>8.3999999999999995E-3</v>
+        <v>5.4999999999999997E-3</v>
       </c>
       <c r="C3">
-        <v>2.8999999999999998E-3</v>
+        <v>1.6999999999999999E-3</v>
       </c>
       <c r="D3">
-        <v>2.5000000000000001E-3</v>
+        <v>1.4E-3</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E9" si="3">SUM(B3:C3)</f>
-        <v>1.1299999999999999E-2</v>
+        <v>7.1999999999999998E-3</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F9" si="4">SUM(B3:D3)</f>
-        <v>1.38E-2</v>
+        <v>8.6E-3</v>
       </c>
       <c r="G3">
-        <v>0.19900000000000001</v>
+        <v>8.5400000000000004E-2</v>
       </c>
       <c r="H3">
-        <v>0.79710000000000003</v>
+        <v>0.3075</v>
       </c>
       <c r="I3">
-        <v>4.9799999999999997E-2</v>
+        <v>5.28E-2</v>
       </c>
       <c r="J3">
-        <v>2.8E-3</v>
+        <v>1.5E-3</v>
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K9" si="5">SUM(G3:H3)</f>
-        <v>0.99609999999999999</v>
+        <v>0.39290000000000003</v>
       </c>
       <c r="L3">
         <f t="shared" si="0"/>
-        <v>1.0487</v>
+        <v>0.44720000000000004</v>
       </c>
       <c r="M3">
-        <v>4.986E-3</v>
+        <v>3.4970000000000001E-3</v>
       </c>
       <c r="N3">
-        <v>1.763E-3</v>
+        <v>1.0859999999999999E-3</v>
       </c>
       <c r="O3">
-        <v>4.3199999999999998E-4</v>
+        <v>2.6600000000000001E-4</v>
       </c>
       <c r="P3">
         <f t="shared" ref="P3:P9" si="6">SUM(M3:N3)</f>
-        <v>6.7489999999999998E-3</v>
+        <v>4.5830000000000003E-3</v>
       </c>
       <c r="Q3">
         <f t="shared" si="1"/>
-        <v>7.1809999999999999E-3</v>
+        <v>4.849E-3</v>
       </c>
       <c r="R3">
-        <v>0.44561600000000001</v>
+        <v>0.19217400000000001</v>
       </c>
       <c r="S3">
-        <v>0.59089499999999995</v>
+        <v>0.21096799999999999</v>
       </c>
       <c r="T3">
-        <v>8.3520999999999998E-2</v>
+        <v>6.3317999999999999E-2</v>
       </c>
       <c r="U3">
-        <v>1.258E-3</v>
+        <v>5.8299999999999997E-4</v>
       </c>
       <c r="V3">
         <f t="shared" ref="V3:V9" si="7">SUM(R3:S3)</f>
-        <v>1.036511</v>
+        <v>0.403142</v>
       </c>
       <c r="W3">
         <f t="shared" si="2"/>
-        <v>1.1212899999999999</v>
+        <v>0.46704299999999999</v>
       </c>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.45">
@@ -8459,78 +7437,78 @@
         <v>1000</v>
       </c>
       <c r="B4">
-        <v>8.5900000000000004E-2</v>
+        <v>4.6100000000000002E-2</v>
       </c>
       <c r="C4">
-        <v>1.9E-2</v>
+        <v>1.26E-2</v>
       </c>
       <c r="D4">
-        <v>2.8299999999999999E-2</v>
+        <v>1.34E-2</v>
       </c>
       <c r="E4">
         <f t="shared" si="3"/>
-        <v>0.10490000000000001</v>
+        <v>5.8700000000000002E-2</v>
       </c>
       <c r="F4">
         <f t="shared" si="4"/>
-        <v>0.13320000000000001</v>
+        <v>7.2099999999999997E-2</v>
       </c>
       <c r="G4">
-        <v>0.19900000000000001</v>
+        <v>5.9400000000000001E-2</v>
       </c>
       <c r="H4">
-        <v>1.0247999999999999</v>
+        <v>0.31919999999999998</v>
       </c>
       <c r="I4">
-        <v>6.7199999999999996E-2</v>
+        <v>6.1199999999999997E-2</v>
       </c>
       <c r="J4">
-        <v>2.5000000000000001E-2</v>
+        <v>1.3599999999999999E-2</v>
       </c>
       <c r="K4">
         <f t="shared" si="5"/>
-        <v>1.2238</v>
+        <v>0.37859999999999999</v>
       </c>
       <c r="L4">
         <f t="shared" si="0"/>
-        <v>1.3159999999999998</v>
+        <v>0.45339999999999997</v>
       </c>
       <c r="M4">
-        <v>5.6697999999999998E-2</v>
+        <v>3.4388000000000002E-2</v>
       </c>
       <c r="N4">
-        <v>1.7961999999999999E-2</v>
+        <v>1.1872000000000001E-2</v>
       </c>
       <c r="O4">
-        <v>3.875E-3</v>
+        <v>2.2729999999999998E-3</v>
       </c>
       <c r="P4">
         <f t="shared" si="6"/>
-        <v>7.4660000000000004E-2</v>
+        <v>4.6260000000000003E-2</v>
       </c>
       <c r="Q4">
         <f t="shared" si="1"/>
-        <v>7.8535000000000008E-2</v>
+        <v>4.8533E-2</v>
       </c>
       <c r="R4">
-        <v>0.47459200000000001</v>
+        <v>0.186225</v>
       </c>
       <c r="S4">
-        <v>0.84513199999999999</v>
+        <v>0.24310399999999999</v>
       </c>
       <c r="T4">
-        <v>9.7727999999999995E-2</v>
+        <v>6.6530000000000006E-2</v>
       </c>
       <c r="U4">
-        <v>7.025E-3</v>
+        <v>4.7790000000000003E-3</v>
       </c>
       <c r="V4">
         <f t="shared" si="7"/>
-        <v>1.3197239999999999</v>
+        <v>0.42932899999999996</v>
       </c>
       <c r="W4">
         <f t="shared" si="2"/>
-        <v>1.424477</v>
+        <v>0.50063799999999992</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.45">
@@ -8538,78 +7516,78 @@
         <v>10000</v>
       </c>
       <c r="B5">
-        <v>0.84370000000000001</v>
+        <v>0.43590000000000001</v>
       </c>
       <c r="C5">
-        <v>0.44240000000000002</v>
+        <v>0.1149</v>
       </c>
       <c r="D5">
-        <v>0.2477</v>
+        <v>0.13370000000000001</v>
       </c>
       <c r="E5">
         <f t="shared" si="3"/>
-        <v>1.2861</v>
+        <v>0.55079999999999996</v>
       </c>
       <c r="F5">
         <f t="shared" si="4"/>
-        <v>1.5338000000000001</v>
+        <v>0.6845</v>
       </c>
       <c r="G5">
-        <v>0.2001</v>
+        <v>5.79E-2</v>
       </c>
       <c r="H5">
-        <v>1.2468999999999999</v>
+        <v>0.3659</v>
       </c>
       <c r="I5">
-        <v>8.5800000000000001E-2</v>
+        <v>9.6100000000000005E-2</v>
       </c>
       <c r="J5">
-        <v>0.24779999999999999</v>
+        <v>0.1338</v>
       </c>
       <c r="K5">
         <f t="shared" si="5"/>
-        <v>1.4469999999999998</v>
+        <v>0.42380000000000001</v>
       </c>
       <c r="L5">
         <f t="shared" si="0"/>
-        <v>1.7806</v>
+        <v>0.65370000000000006</v>
       </c>
       <c r="M5">
-        <v>0.54696199999999995</v>
+        <v>0.331374</v>
       </c>
       <c r="N5">
-        <v>0.1709</v>
+        <v>0.12942100000000001</v>
       </c>
       <c r="O5">
-        <v>3.5851000000000001E-2</v>
+        <v>2.4208E-2</v>
       </c>
       <c r="P5">
         <f t="shared" si="6"/>
-        <v>0.717862</v>
+        <v>0.46079500000000001</v>
       </c>
       <c r="Q5">
         <f t="shared" si="1"/>
-        <v>0.75371299999999997</v>
+        <v>0.48500300000000002</v>
       </c>
       <c r="R5">
-        <v>0.47682099999999999</v>
+        <v>0.203847</v>
       </c>
       <c r="S5">
-        <v>0.82023599999999997</v>
+        <v>0.29677300000000001</v>
       </c>
       <c r="T5">
-        <v>0.105322</v>
+        <v>8.2985000000000003E-2</v>
       </c>
       <c r="U5">
-        <v>6.5559000000000006E-2</v>
+        <v>5.4524999999999997E-2</v>
       </c>
       <c r="V5">
         <f t="shared" si="7"/>
-        <v>1.2970569999999999</v>
+        <v>0.50062000000000006</v>
       </c>
       <c r="W5">
         <f t="shared" si="2"/>
-        <v>1.4679379999999997</v>
+        <v>0.63813000000000009</v>
       </c>
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.45">
@@ -8617,78 +7595,78 @@
         <v>100000</v>
       </c>
       <c r="B6">
-        <v>8.7974999999999994</v>
+        <v>4.6462000000000003</v>
       </c>
       <c r="C6">
-        <v>2.4841000000000002</v>
+        <v>1.2143999999999999</v>
       </c>
       <c r="D6">
-        <v>2.4857999999999998</v>
+        <v>1.4245000000000001</v>
       </c>
       <c r="E6">
         <f t="shared" si="3"/>
-        <v>11.281599999999999</v>
+        <v>5.8605999999999998</v>
       </c>
       <c r="F6">
         <f t="shared" si="4"/>
-        <v>13.767399999999999</v>
+        <v>7.2850999999999999</v>
       </c>
       <c r="G6">
-        <v>0.22470000000000001</v>
+        <v>6.0600000000000001E-2</v>
       </c>
       <c r="H6">
-        <v>2.9426999999999999</v>
+        <v>1.2386999999999999</v>
       </c>
       <c r="I6">
-        <v>2.0160999999999998</v>
+        <v>0.51359999999999995</v>
       </c>
       <c r="J6">
-        <v>2.4756999999999998</v>
+        <v>1.3708</v>
       </c>
       <c r="K6">
         <f t="shared" si="5"/>
-        <v>3.1673999999999998</v>
+        <v>1.2992999999999999</v>
       </c>
       <c r="L6">
         <f t="shared" si="0"/>
-        <v>7.6591999999999993</v>
+        <v>3.1837</v>
       </c>
       <c r="M6">
-        <v>5.46922</v>
+        <v>3.3493400000000002</v>
       </c>
       <c r="N6">
-        <v>1.97777</v>
+        <v>1.3481300000000001</v>
       </c>
       <c r="O6">
-        <v>0.34337899999999999</v>
+        <v>0.23305300000000001</v>
       </c>
       <c r="P6">
         <f t="shared" si="6"/>
-        <v>7.4469899999999996</v>
+        <v>4.69747</v>
       </c>
       <c r="Q6">
         <f t="shared" si="1"/>
-        <v>7.7903689999999992</v>
+        <v>4.930523</v>
       </c>
       <c r="R6">
-        <v>0.37850499999999998</v>
+        <v>0.18995100000000001</v>
       </c>
       <c r="S6">
-        <v>2.9758</v>
+        <v>1.48854</v>
       </c>
       <c r="T6">
-        <v>0.464864</v>
+        <v>0.31885000000000002</v>
       </c>
       <c r="U6">
-        <v>0.69070699999999996</v>
+        <v>0.47934500000000002</v>
       </c>
       <c r="V6">
         <f t="shared" si="7"/>
-        <v>3.3543050000000001</v>
+        <v>1.678491</v>
       </c>
       <c r="W6">
         <f t="shared" si="2"/>
-        <v>4.5098760000000002</v>
+        <v>2.4766859999999999</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.45">
@@ -8696,78 +7674,78 @@
         <v>1000000</v>
       </c>
       <c r="B7">
-        <v>73.321100000000001</v>
+        <v>41.9816</v>
       </c>
       <c r="C7">
-        <v>21.799900000000001</v>
+        <v>15.0382</v>
       </c>
       <c r="D7">
-        <v>23.4847</v>
+        <v>12.792</v>
       </c>
       <c r="E7">
         <f t="shared" si="3"/>
-        <v>95.121000000000009</v>
+        <v>57.019800000000004</v>
       </c>
       <c r="F7">
         <f t="shared" si="4"/>
-        <v>118.60570000000001</v>
+        <v>69.811800000000005</v>
       </c>
       <c r="G7">
-        <v>0.47810000000000002</v>
+        <v>0.17019999999999999</v>
       </c>
       <c r="H7">
-        <v>5.0983999999999998</v>
+        <v>5.6425000000000001</v>
       </c>
       <c r="I7">
-        <v>4.6943999999999999</v>
+        <v>4.1814999999999998</v>
       </c>
       <c r="J7">
-        <v>25.093299999999999</v>
+        <v>12.843299999999999</v>
       </c>
       <c r="K7">
         <f t="shared" si="5"/>
-        <v>5.5765000000000002</v>
+        <v>5.8127000000000004</v>
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>35.364199999999997</v>
+        <v>22.837499999999999</v>
       </c>
       <c r="M7">
-        <v>46.990099999999998</v>
+        <v>31.771699999999999</v>
       </c>
       <c r="N7">
-        <v>16.2499</v>
+        <v>15.199400000000001</v>
       </c>
       <c r="O7">
-        <v>3.2206899999999998</v>
+        <v>2.6561699999999999</v>
       </c>
       <c r="P7">
         <f t="shared" si="6"/>
-        <v>63.239999999999995</v>
+        <v>46.9711</v>
       </c>
       <c r="Q7">
         <f t="shared" si="1"/>
-        <v>66.46069</v>
+        <v>49.627270000000003</v>
       </c>
       <c r="R7">
-        <v>1.00038</v>
+        <v>0.40144400000000002</v>
       </c>
       <c r="S7">
-        <v>6.0666500000000001</v>
+        <v>5.6603300000000001</v>
       </c>
       <c r="T7">
-        <v>5.2098500000000003</v>
+        <v>5.20688</v>
       </c>
       <c r="U7">
-        <v>6.5240200000000002</v>
+        <v>4.4508200000000002</v>
       </c>
       <c r="V7">
         <f t="shared" si="7"/>
-        <v>7.0670299999999999</v>
+        <v>6.0617739999999998</v>
       </c>
       <c r="W7">
         <f t="shared" si="2"/>
-        <v>18.800899999999999</v>
+        <v>15.719474</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.45">
@@ -8775,78 +7753,78 @@
         <v>10000000</v>
       </c>
       <c r="B8">
-        <v>624.23699999999997</v>
+        <v>412.77499999999998</v>
       </c>
       <c r="C8">
-        <v>188.989</v>
+        <v>149.72</v>
       </c>
       <c r="D8">
-        <v>209.03200000000001</v>
+        <v>127.27500000000001</v>
       </c>
       <c r="E8">
         <f t="shared" si="3"/>
-        <v>813.226</v>
+        <v>562.495</v>
       </c>
       <c r="F8">
         <f t="shared" si="4"/>
-        <v>1022.258</v>
+        <v>689.77</v>
       </c>
       <c r="G8">
-        <v>0.98419999999999996</v>
+        <v>0.92459999999999998</v>
       </c>
       <c r="H8">
-        <v>29.4176</v>
+        <v>44.822099999999999</v>
       </c>
       <c r="I8">
-        <v>42.903700000000001</v>
+        <v>39.967799999999997</v>
       </c>
       <c r="J8">
-        <v>225.434</v>
+        <v>127.074</v>
       </c>
       <c r="K8">
         <f t="shared" si="5"/>
-        <v>30.401800000000001</v>
+        <v>45.746699999999997</v>
       </c>
       <c r="L8">
         <f t="shared" si="0"/>
-        <v>298.73950000000002</v>
+        <v>212.7885</v>
       </c>
       <c r="M8">
-        <v>458.85199999999998</v>
+        <v>307.89400000000001</v>
       </c>
       <c r="N8">
-        <v>167.935</v>
+        <v>127.69</v>
       </c>
       <c r="O8">
-        <v>33.293500000000002</v>
+        <v>22.965199999999999</v>
       </c>
       <c r="P8">
         <f t="shared" si="6"/>
-        <v>626.78700000000003</v>
+        <v>435.584</v>
       </c>
       <c r="Q8">
         <f t="shared" si="1"/>
-        <v>660.08050000000003</v>
+        <v>458.54919999999998</v>
       </c>
       <c r="R8">
-        <v>2.84823</v>
+        <v>1.5768500000000001</v>
       </c>
       <c r="S8">
-        <v>27.171700000000001</v>
+        <v>43.444499999999998</v>
       </c>
       <c r="T8">
-        <v>46.458199999999998</v>
+        <v>47.012700000000002</v>
       </c>
       <c r="U8">
-        <v>65.723500000000001</v>
+        <v>43.414999999999999</v>
       </c>
       <c r="V8">
         <f t="shared" si="7"/>
-        <v>30.019930000000002</v>
+        <v>45.021349999999998</v>
       </c>
       <c r="W8">
         <f t="shared" si="2"/>
-        <v>142.20162999999999</v>
+        <v>135.44905</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.45">
@@ -8854,78 +7832,820 @@
         <v>100000000</v>
       </c>
       <c r="B9">
-        <v>6345.27</v>
+        <v>4283.7299999999996</v>
       </c>
       <c r="C9">
-        <v>2010.93</v>
+        <v>1427.25</v>
       </c>
       <c r="D9">
-        <v>2106.0100000000002</v>
+        <v>1278.49</v>
       </c>
       <c r="E9">
         <f t="shared" si="3"/>
-        <v>8356.2000000000007</v>
+        <v>5710.98</v>
       </c>
       <c r="F9">
         <f t="shared" si="4"/>
-        <v>10462.210000000001</v>
+        <v>6989.4699999999993</v>
       </c>
       <c r="G9">
-        <v>7.2793000000000001</v>
+        <v>2.8048999999999999</v>
       </c>
       <c r="H9">
-        <v>260.947</v>
+        <v>405.38400000000001</v>
       </c>
       <c r="I9">
-        <v>373.25200000000001</v>
+        <v>400.85500000000002</v>
       </c>
       <c r="J9">
-        <v>2340.81</v>
+        <v>1301.2</v>
       </c>
       <c r="K9">
         <f t="shared" si="5"/>
-        <v>268.22629999999998</v>
+        <v>408.18889999999999</v>
       </c>
       <c r="L9">
         <f t="shared" si="0"/>
-        <v>2982.2883000000002</v>
+        <v>2110.2438999999999</v>
       </c>
       <c r="M9">
-        <v>4632.47</v>
+        <v>3130.81</v>
       </c>
       <c r="N9">
-        <v>4517.74</v>
+        <v>1366.69</v>
       </c>
       <c r="O9">
-        <v>328.387</v>
+        <v>248.45500000000001</v>
       </c>
       <c r="P9">
         <f t="shared" si="6"/>
-        <v>9150.2099999999991</v>
+        <v>4497.5</v>
       </c>
       <c r="Q9">
         <f t="shared" si="1"/>
-        <v>9478.5969999999998</v>
+        <v>4745.9549999999999</v>
       </c>
       <c r="R9">
-        <v>16.939800000000002</v>
+        <v>7.3137499999999998</v>
       </c>
       <c r="S9">
-        <v>235.39599999999999</v>
+        <v>408.22899999999998</v>
       </c>
       <c r="T9">
-        <v>431.298</v>
+        <v>547.71600000000001</v>
       </c>
       <c r="U9">
-        <v>647.99900000000002</v>
+        <v>449.26600000000002</v>
       </c>
       <c r="V9">
         <f t="shared" si="7"/>
-        <v>252.33579999999998</v>
+        <v>415.54275000000001</v>
       </c>
       <c r="W9">
         <f t="shared" si="2"/>
-        <v>1331.6327999999999</v>
+        <v>1412.52475</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CF9CBA4-1D0E-4C7D-85A3-E5E8BE03303C}">
+  <dimension ref="A1:W9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <cols>
+    <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.19921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.53125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.53125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.59765625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.796875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.19921875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.9296875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.19921875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.19921875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.86328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.3984375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.53125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.59765625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.59765625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.796875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.19921875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.796875" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.9296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A2" s="1">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="C2">
+        <v>1.1000000000000001E-3</v>
+      </c>
+      <c r="D2">
+        <v>4.0000000000000002E-4</v>
+      </c>
+      <c r="E2">
+        <f>SUM(B2:C2)</f>
+        <v>1.21E-2</v>
+      </c>
+      <c r="F2">
+        <f>SUM(B2:D2)</f>
+        <v>1.2499999999999999E-2</v>
+      </c>
+      <c r="G2">
+        <v>0.36609999999999998</v>
+      </c>
+      <c r="H2">
+        <v>0.44450000000000001</v>
+      </c>
+      <c r="I2">
+        <v>5.21E-2</v>
+      </c>
+      <c r="J2">
+        <v>5.9999999999999995E-4</v>
+      </c>
+      <c r="K2">
+        <f>SUM(G2:H2)</f>
+        <v>0.81059999999999999</v>
+      </c>
+      <c r="L2">
+        <f t="shared" ref="L2:L9" si="0">SUM(G2:J2)</f>
+        <v>0.86330000000000007</v>
+      </c>
+      <c r="M2">
+        <v>1.0893999999999999E-2</v>
+      </c>
+      <c r="N2">
+        <v>8.9700000000000001E-4</v>
+      </c>
+      <c r="O2">
+        <v>2.3000000000000001E-4</v>
+      </c>
+      <c r="P2">
+        <f>SUM(M2:N2)</f>
+        <v>1.1790999999999999E-2</v>
+      </c>
+      <c r="Q2">
+        <f t="shared" ref="Q2:Q9" si="1">SUM(M2:O2)</f>
+        <v>1.2020999999999999E-2</v>
+      </c>
+      <c r="R2">
+        <v>0.78912199999999999</v>
+      </c>
+      <c r="S2">
+        <v>0.48511300000000002</v>
+      </c>
+      <c r="T2">
+        <v>9.3202999999999994E-2</v>
+      </c>
+      <c r="U2">
+        <v>7.5699999999999997E-4</v>
+      </c>
+      <c r="V2">
+        <f>SUM(R2:S2)</f>
+        <v>1.274235</v>
+      </c>
+      <c r="W2">
+        <f t="shared" ref="W2:W9" si="2">SUM(R2:U2)</f>
+        <v>1.3681949999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A3" s="1">
+        <v>100</v>
+      </c>
+      <c r="B3">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="C3">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="D3">
+        <v>2.2000000000000001E-3</v>
+      </c>
+      <c r="E3">
+        <f t="shared" ref="E3:E9" si="3">SUM(B3:C3)</f>
+        <v>1.3399999999999999E-2</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F9" si="4">SUM(B3:D3)</f>
+        <v>1.5599999999999999E-2</v>
+      </c>
+      <c r="G3">
+        <v>0.374</v>
+      </c>
+      <c r="H3">
+        <v>0.5595</v>
+      </c>
+      <c r="I3">
+        <v>4.5100000000000001E-2</v>
+      </c>
+      <c r="J3">
+        <v>2.3999999999999998E-3</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K9" si="5">SUM(G3:H3)</f>
+        <v>0.9335</v>
+      </c>
+      <c r="L3">
+        <f t="shared" si="0"/>
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="M3">
+        <v>6.0200000000000002E-3</v>
+      </c>
+      <c r="N3">
+        <v>1.5950000000000001E-3</v>
+      </c>
+      <c r="O3">
+        <v>1.4649999999999999E-3</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P9" si="6">SUM(M3:N3)</f>
+        <v>7.6150000000000002E-3</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" si="1"/>
+        <v>9.0799999999999995E-3</v>
+      </c>
+      <c r="R3">
+        <v>0.79770399999999997</v>
+      </c>
+      <c r="S3">
+        <v>0.72060800000000003</v>
+      </c>
+      <c r="T3">
+        <v>0.11562</v>
+      </c>
+      <c r="U3">
+        <v>1.6149999999999999E-3</v>
+      </c>
+      <c r="V3">
+        <f t="shared" ref="V3:V9" si="7">SUM(R3:S3)</f>
+        <v>1.5183119999999999</v>
+      </c>
+      <c r="W3">
+        <f t="shared" si="2"/>
+        <v>1.6355469999999999</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A4" s="1">
+        <v>1000</v>
+      </c>
+      <c r="B4">
+        <v>6.6900000000000001E-2</v>
+      </c>
+      <c r="C4">
+        <v>1.5800000000000002E-2</v>
+      </c>
+      <c r="D4">
+        <v>2.24E-2</v>
+      </c>
+      <c r="E4">
+        <f t="shared" si="3"/>
+        <v>8.2699999999999996E-2</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="4"/>
+        <v>0.1051</v>
+      </c>
+      <c r="G4">
+        <v>0.35499999999999998</v>
+      </c>
+      <c r="H4">
+        <v>0.81599999999999995</v>
+      </c>
+      <c r="I4">
+        <v>4.9700000000000001E-2</v>
+      </c>
+      <c r="J4">
+        <v>2.1999999999999999E-2</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="5"/>
+        <v>1.1709999999999998</v>
+      </c>
+      <c r="L4">
+        <f t="shared" si="0"/>
+        <v>1.2426999999999999</v>
+      </c>
+      <c r="M4">
+        <v>5.0095000000000001E-2</v>
+      </c>
+      <c r="N4">
+        <v>1.4134000000000001E-2</v>
+      </c>
+      <c r="O4">
+        <v>1.4264000000000001E-2</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="6"/>
+        <v>6.4229000000000008E-2</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="1"/>
+        <v>7.8493000000000007E-2</v>
+      </c>
+      <c r="R4">
+        <v>0.76904399999999995</v>
+      </c>
+      <c r="S4">
+        <v>0.81545599999999996</v>
+      </c>
+      <c r="T4">
+        <v>0.108473</v>
+      </c>
+      <c r="U4">
+        <v>1.5180000000000001E-2</v>
+      </c>
+      <c r="V4">
+        <f t="shared" si="7"/>
+        <v>1.5844999999999998</v>
+      </c>
+      <c r="W4">
+        <f t="shared" si="2"/>
+        <v>1.7081529999999998</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A5" s="1">
+        <v>10000</v>
+      </c>
+      <c r="B5">
+        <v>0.87680000000000002</v>
+      </c>
+      <c r="C5">
+        <v>0.3977</v>
+      </c>
+      <c r="D5">
+        <v>0.22600000000000001</v>
+      </c>
+      <c r="E5">
+        <f t="shared" si="3"/>
+        <v>1.2745</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="4"/>
+        <v>1.5004999999999999</v>
+      </c>
+      <c r="G5">
+        <v>0.34970000000000001</v>
+      </c>
+      <c r="H5">
+        <v>1.0562</v>
+      </c>
+      <c r="I5">
+        <v>8.77E-2</v>
+      </c>
+      <c r="J5">
+        <v>0.2162</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="5"/>
+        <v>1.4058999999999999</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="0"/>
+        <v>1.7097999999999998</v>
+      </c>
+      <c r="M5">
+        <v>0.48528199999999999</v>
+      </c>
+      <c r="N5">
+        <v>0.16278400000000001</v>
+      </c>
+      <c r="O5">
+        <v>0.14236099999999999</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="6"/>
+        <v>0.64806600000000003</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="1"/>
+        <v>0.79042699999999999</v>
+      </c>
+      <c r="R5">
+        <v>0.73763199999999995</v>
+      </c>
+      <c r="S5">
+        <v>1.0383199999999999</v>
+      </c>
+      <c r="T5">
+        <v>0.13372999999999999</v>
+      </c>
+      <c r="U5">
+        <v>0.15206900000000001</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="7"/>
+        <v>1.7759519999999998</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="2"/>
+        <v>2.0617509999999997</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A6" s="1">
+        <v>100000</v>
+      </c>
+      <c r="B6">
+        <v>8.2843999999999998</v>
+      </c>
+      <c r="C6">
+        <v>2.8515000000000001</v>
+      </c>
+      <c r="D6">
+        <v>2.1312000000000002</v>
+      </c>
+      <c r="E6">
+        <f t="shared" si="3"/>
+        <v>11.135899999999999</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="4"/>
+        <v>13.267099999999999</v>
+      </c>
+      <c r="G6">
+        <v>0.64990000000000003</v>
+      </c>
+      <c r="H6">
+        <v>1.2072000000000001</v>
+      </c>
+      <c r="I6">
+        <v>1.7783</v>
+      </c>
+      <c r="J6">
+        <v>2.1878000000000002</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="5"/>
+        <v>1.8571</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="0"/>
+        <v>5.8231999999999999</v>
+      </c>
+      <c r="M6">
+        <v>5.5338000000000003</v>
+      </c>
+      <c r="N6">
+        <v>1.5807199999999999</v>
+      </c>
+      <c r="O6">
+        <v>1.4047799999999999</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="6"/>
+        <v>7.1145200000000006</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="1"/>
+        <v>8.5193000000000012</v>
+      </c>
+      <c r="R6">
+        <v>1.49779</v>
+      </c>
+      <c r="S6">
+        <v>1.0183500000000001</v>
+      </c>
+      <c r="T6">
+        <v>0.74007299999999998</v>
+      </c>
+      <c r="U6">
+        <v>1.5267500000000001</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="7"/>
+        <v>2.51614</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="2"/>
+        <v>4.7829629999999996</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A7" s="1">
+        <v>1000000</v>
+      </c>
+      <c r="B7">
+        <v>65.916799999999995</v>
+      </c>
+      <c r="C7">
+        <v>20.0382</v>
+      </c>
+      <c r="D7">
+        <v>23.014099999999999</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="3"/>
+        <v>85.954999999999998</v>
+      </c>
+      <c r="F7">
+        <f t="shared" si="4"/>
+        <v>108.9691</v>
+      </c>
+      <c r="G7">
+        <v>1.9619</v>
+      </c>
+      <c r="H7">
+        <v>4.0708000000000002</v>
+      </c>
+      <c r="I7">
+        <v>4.1185</v>
+      </c>
+      <c r="J7">
+        <v>21.2867</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="5"/>
+        <v>6.0327000000000002</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="0"/>
+        <v>31.437899999999999</v>
+      </c>
+      <c r="M7">
+        <v>58.444699999999997</v>
+      </c>
+      <c r="N7">
+        <v>15.230600000000001</v>
+      </c>
+      <c r="O7">
+        <v>16.532299999999999</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="6"/>
+        <v>73.675299999999993</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="1"/>
+        <v>90.207599999999985</v>
+      </c>
+      <c r="R7">
+        <v>2.3258800000000002</v>
+      </c>
+      <c r="S7">
+        <v>6.4141000000000004</v>
+      </c>
+      <c r="T7">
+        <v>5.8773900000000001</v>
+      </c>
+      <c r="U7">
+        <v>14.942600000000001</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="7"/>
+        <v>8.739980000000001</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="2"/>
+        <v>29.55997</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A8" s="1">
+        <v>10000000</v>
+      </c>
+      <c r="B8">
+        <v>674.26099999999997</v>
+      </c>
+      <c r="C8">
+        <v>221.881</v>
+      </c>
+      <c r="D8">
+        <v>244.983</v>
+      </c>
+      <c r="E8">
+        <f t="shared" si="3"/>
+        <v>896.14199999999994</v>
+      </c>
+      <c r="F8">
+        <f t="shared" si="4"/>
+        <v>1141.125</v>
+      </c>
+      <c r="G8">
+        <v>13.712899999999999</v>
+      </c>
+      <c r="H8">
+        <v>21.736799999999999</v>
+      </c>
+      <c r="I8">
+        <v>36.780700000000003</v>
+      </c>
+      <c r="J8">
+        <v>218.20400000000001</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="5"/>
+        <v>35.4497</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="0"/>
+        <v>290.43439999999998</v>
+      </c>
+      <c r="M8">
+        <v>537.09900000000005</v>
+      </c>
+      <c r="N8">
+        <v>155.815</v>
+      </c>
+      <c r="O8">
+        <v>135.732</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="6"/>
+        <v>692.91399999999999</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="1"/>
+        <v>828.64599999999996</v>
+      </c>
+      <c r="R8">
+        <v>14.3728</v>
+      </c>
+      <c r="S8">
+        <v>22.856100000000001</v>
+      </c>
+      <c r="T8">
+        <v>50.585000000000001</v>
+      </c>
+      <c r="U8">
+        <v>165.07599999999999</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="7"/>
+        <v>37.228900000000003</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="2"/>
+        <v>252.88990000000001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.45">
+      <c r="A9" s="1">
+        <v>100000000</v>
+      </c>
+      <c r="B9">
+        <v>6572.32</v>
+      </c>
+      <c r="C9">
+        <v>1993.29</v>
+      </c>
+      <c r="D9">
+        <v>2276.71</v>
+      </c>
+      <c r="E9">
+        <f t="shared" si="3"/>
+        <v>8565.61</v>
+      </c>
+      <c r="F9">
+        <f t="shared" si="4"/>
+        <v>10842.32</v>
+      </c>
+      <c r="G9">
+        <v>122.96</v>
+      </c>
+      <c r="H9">
+        <v>177.33699999999999</v>
+      </c>
+      <c r="I9">
+        <v>381.62700000000001</v>
+      </c>
+      <c r="J9">
+        <v>2216.34</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="5"/>
+        <v>300.29699999999997</v>
+      </c>
+      <c r="L9">
+        <f t="shared" si="0"/>
+        <v>2898.2640000000001</v>
+      </c>
+      <c r="M9">
+        <v>5212.12</v>
+      </c>
+      <c r="N9">
+        <v>1649.66</v>
+      </c>
+      <c r="O9">
+        <v>1451.85</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="6"/>
+        <v>6861.78</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="1"/>
+        <v>8313.6299999999992</v>
+      </c>
+      <c r="R9">
+        <v>131.31</v>
+      </c>
+      <c r="S9">
+        <v>188.95</v>
+      </c>
+      <c r="T9">
+        <v>502.19400000000002</v>
+      </c>
+      <c r="U9">
+        <v>1449.93</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="7"/>
+        <v>320.26</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="2"/>
+        <v>2272.384</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updates to performance measurements
</commit_message>
<xml_diff>
--- a/docs/performance.xlsx
+++ b/docs/performance.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27726"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/22e8633286bd19a7/Documents/dev/map-reduce/docs/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ngc-my.sharepoint.us/personal/harold_andrews_ngc_com/Documents/Documents/dev/map-reduce.ng/docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="241" documentId="8_{8E589E63-48AD-4E69-8076-DD012BDE5EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A335181C-6024-4FB4-BCDA-B3B864BF376D}"/>
+  <xr:revisionPtr revIDLastSave="245" documentId="8_{8E589E63-48AD-4E69-8076-DD012BDE5EAA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4B8BFA00-0CFC-4F27-82E2-F2FB1615A685}"/>
   <bookViews>
-    <workbookView xWindow="28702" yWindow="-98" windowWidth="28995" windowHeight="15675" activeTab="1" xr2:uid="{9DF68624-D4B9-4083-BFAE-DE2CA7971FFA}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{9DF68624-D4B9-4083-BFAE-DE2CA7971FFA}"/>
   </bookViews>
   <sheets>
     <sheet name="Intel CPU" sheetId="1" r:id="rId1"/>
@@ -113,7 +113,7 @@
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -591,10 +591,9 @@
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -813,28 +812,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>4.7999999999999996E-3</c:v>
+                  <c:v>7.1999999999999998E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.6E-3</c:v>
+                  <c:v>1.0700000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.2099999999999997E-2</c:v>
+                  <c:v>7.2899999999999993E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.6845</c:v>
+                  <c:v>0.70610000000000006</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.2850999999999999</c:v>
+                  <c:v>7.4606000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>69.811800000000005</c:v>
+                  <c:v>71.044700000000006</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>689.77</c:v>
+                  <c:v>719.09100000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6989.4699999999993</c:v>
+                  <c:v>7413.4400000000005</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -930,28 +929,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.41709999999999997</c:v>
+                  <c:v>0.4511</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.44720000000000004</c:v>
+                  <c:v>0.46650000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.45339999999999997</c:v>
+                  <c:v>0.52179999999999993</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.65370000000000006</c:v>
+                  <c:v>0.71860000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.1837</c:v>
+                  <c:v>2.7069999999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>22.837499999999999</c:v>
+                  <c:v>23.921799999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>212.7885</c:v>
+                  <c:v>222.27449999999999</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2110.2438999999999</c:v>
+                  <c:v>2222.7530000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1041,28 +1040,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>7.8100000000000001E-3</c:v>
+                  <c:v>1.3313E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.849E-3</c:v>
+                  <c:v>7.8399999999999997E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.8533E-2</c:v>
+                  <c:v>5.6257999999999996E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.48500300000000002</c:v>
+                  <c:v>0.54588199999999998</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.930523</c:v>
+                  <c:v>5.5287470000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>49.627270000000003</c:v>
+                  <c:v>54.297370000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>458.54919999999998</c:v>
+                  <c:v>587.86329999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4745.9549999999999</c:v>
+                  <c:v>5576.0619999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1152,28 +1151,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.45801800000000004</c:v>
+                  <c:v>0.50641899999999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.46704299999999999</c:v>
+                  <c:v>0.52193600000000007</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.50063799999999992</c:v>
+                  <c:v>0.52859800000000001</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.63813000000000009</c:v>
+                  <c:v>0.6728940000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>2.4766859999999999</c:v>
+                  <c:v>2.3987150000000002</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>15.719474</c:v>
+                  <c:v>21.505769999999998</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>135.44905</c:v>
+                  <c:v>185.09010000000001</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1412.52475</c:v>
+                  <c:v>1958.1369999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1677,28 +1676,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>4.4999999999999997E-3</c:v>
+                  <c:v>6.8999999999999999E-3</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7.1999999999999998E-3</c:v>
+                  <c:v>9.300000000000001E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>5.8700000000000002E-2</c:v>
+                  <c:v>5.9499999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.55079999999999996</c:v>
+                  <c:v>0.57240000000000002</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>5.8605999999999998</c:v>
+                  <c:v>6.1241000000000003</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>57.019800000000004</c:v>
+                  <c:v>57.2393</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>562.495</c:v>
+                  <c:v>590.43600000000004</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>5710.98</c:v>
+                  <c:v>6112.06</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1794,28 +1793,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.34719999999999995</c:v>
+                  <c:v>0.39200000000000002</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.39290000000000003</c:v>
+                  <c:v>0.41250000000000003</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.37859999999999999</c:v>
+                  <c:v>0.44569999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.42380000000000001</c:v>
+                  <c:v>0.49690000000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.2992999999999999</c:v>
+                  <c:v>0.81689999999999996</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5.8127000000000004</c:v>
+                  <c:v>6.4569000000000001</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45.746699999999997</c:v>
+                  <c:v>50.3048</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>408.18889999999999</c:v>
+                  <c:v>440.52800000000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1905,28 +1904,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>7.7260000000000002E-3</c:v>
+                  <c:v>1.3062000000000001E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4.5830000000000003E-3</c:v>
+                  <c:v>6.862E-3</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.6260000000000003E-2</c:v>
+                  <c:v>4.6913999999999997E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.46079500000000001</c:v>
+                  <c:v>0.45260400000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4.69747</c:v>
+                  <c:v>4.6376200000000001</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>46.9711</c:v>
+                  <c:v>45.8765</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>435.584</c:v>
+                  <c:v>491.52499999999998</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4497.5</c:v>
+                  <c:v>4688.6000000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2016,28 +2015,28 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="8"/>
                 <c:pt idx="0">
-                  <c:v>0.39549500000000004</c:v>
+                  <c:v>0.44594199999999995</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.403142</c:v>
+                  <c:v>0.458623</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.42932899999999996</c:v>
+                  <c:v>0.457484</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.50062000000000006</c:v>
+                  <c:v>0.50114100000000006</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>1.678491</c:v>
+                  <c:v>0.96227099999999999</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6.0617739999999998</c:v>
+                  <c:v>7.3568999999999996</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>45.021349999999998</c:v>
+                  <c:v>50.3048</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>415.54275000000001</c:v>
+                  <c:v>445.97900000000004</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6851,10 +6850,6 @@
 </c:userShapes>
 </file>
 
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -7174,36 +7169,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE75E16D-024E-4063-A895-F36D0968513C}">
   <dimension ref="A1:W9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.53125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.53125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.19921875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.9296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.19921875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.19921875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.53125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.19921875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.9296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.8125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.8125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.1875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.8125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.9375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.1875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.1875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.8125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.1875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.8125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.9375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:23">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -7274,636 +7269,636 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:23">
       <c r="A2" s="1">
         <v>10</v>
       </c>
       <c r="B2">
-        <v>3.3999999999999998E-3</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="C2">
-        <v>1.1000000000000001E-3</v>
+        <v>8.9999999999999998E-4</v>
       </c>
       <c r="D2">
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="E2">
         <f>SUM(B2:C2)</f>
-        <v>4.4999999999999997E-3</v>
+        <v>6.8999999999999999E-3</v>
       </c>
       <c r="F2">
         <f>SUM(B2:D2)</f>
-        <v>4.7999999999999996E-3</v>
+        <v>7.1999999999999998E-3</v>
       </c>
       <c r="G2">
-        <v>8.7499999999999994E-2</v>
+        <v>0.25900000000000001</v>
       </c>
       <c r="H2">
-        <v>0.25969999999999999</v>
+        <v>0.13300000000000001</v>
       </c>
       <c r="I2">
-        <v>6.1400000000000003E-2</v>
+        <v>5.8700000000000002E-2</v>
       </c>
       <c r="J2">
-        <v>8.5000000000000006E-3</v>
+        <v>4.0000000000000002E-4</v>
       </c>
       <c r="K2">
         <f>SUM(G2:H2)</f>
-        <v>0.34719999999999995</v>
+        <v>0.39200000000000002</v>
       </c>
       <c r="L2">
         <f t="shared" ref="L2:L9" si="0">SUM(G2:J2)</f>
-        <v>0.41709999999999997</v>
+        <v>0.4511</v>
       </c>
       <c r="M2">
-        <v>6.718E-3</v>
+        <v>1.0070000000000001E-2</v>
       </c>
       <c r="N2">
-        <v>1.008E-3</v>
-      </c>
-      <c r="O2" s="2">
-        <v>8.3999999999999995E-5</v>
+        <v>2.9919999999999999E-3</v>
+      </c>
+      <c r="O2">
+        <v>2.5099999999999998E-4</v>
       </c>
       <c r="P2">
         <f>SUM(M2:N2)</f>
-        <v>7.7260000000000002E-3</v>
+        <v>1.3062000000000001E-2</v>
       </c>
       <c r="Q2">
         <f t="shared" ref="Q2:Q9" si="1">SUM(M2:O2)</f>
-        <v>7.8100000000000001E-3</v>
+        <v>1.3313E-2</v>
       </c>
       <c r="R2">
-        <v>0.20544100000000001</v>
+        <v>0.29376799999999997</v>
       </c>
       <c r="S2">
-        <v>0.190054</v>
+        <v>0.152174</v>
       </c>
       <c r="T2">
-        <v>6.2382E-2</v>
+        <v>6.0156000000000001E-2</v>
       </c>
       <c r="U2">
-        <v>1.4100000000000001E-4</v>
+        <v>3.21E-4</v>
       </c>
       <c r="V2">
         <f>SUM(R2:S2)</f>
-        <v>0.39549500000000004</v>
+        <v>0.44594199999999995</v>
       </c>
       <c r="W2">
         <f t="shared" ref="W2:W9" si="2">SUM(R2:U2)</f>
-        <v>0.45801800000000004</v>
+        <v>0.50641899999999995</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:23">
       <c r="A3" s="1">
         <v>100</v>
       </c>
       <c r="B3">
-        <v>5.4999999999999997E-3</v>
+        <v>7.7000000000000002E-3</v>
       </c>
       <c r="C3">
-        <v>1.6999999999999999E-3</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="D3">
         <v>1.4E-3</v>
       </c>
       <c r="E3">
         <f t="shared" ref="E3:E9" si="3">SUM(B3:C3)</f>
-        <v>7.1999999999999998E-3</v>
+        <v>9.300000000000001E-3</v>
       </c>
       <c r="F3">
         <f t="shared" ref="F3:F9" si="4">SUM(B3:D3)</f>
-        <v>8.6E-3</v>
+        <v>1.0700000000000001E-2</v>
       </c>
       <c r="G3">
-        <v>8.5400000000000004E-2</v>
+        <v>0.25380000000000003</v>
       </c>
       <c r="H3">
-        <v>0.3075</v>
+        <v>0.15870000000000001</v>
       </c>
       <c r="I3">
-        <v>5.28E-2</v>
+        <v>5.2400000000000002E-2</v>
       </c>
       <c r="J3">
-        <v>1.5E-3</v>
+        <v>1.6000000000000001E-3</v>
       </c>
       <c r="K3">
         <f t="shared" ref="K3:K9" si="5">SUM(G3:H3)</f>
-        <v>0.39290000000000003</v>
+        <v>0.41250000000000003</v>
       </c>
       <c r="L3">
         <f t="shared" si="0"/>
-        <v>0.44720000000000004</v>
+        <v>0.46650000000000003</v>
       </c>
       <c r="M3">
-        <v>3.4970000000000001E-3</v>
+        <v>5.64E-3</v>
       </c>
       <c r="N3">
-        <v>1.0859999999999999E-3</v>
+        <v>1.222E-3</v>
       </c>
       <c r="O3">
-        <v>2.6600000000000001E-4</v>
+        <v>9.7799999999999992E-4</v>
       </c>
       <c r="P3">
         <f t="shared" ref="P3:P9" si="6">SUM(M3:N3)</f>
-        <v>4.5830000000000003E-3</v>
+        <v>6.862E-3</v>
       </c>
       <c r="Q3">
         <f t="shared" si="1"/>
-        <v>4.849E-3</v>
+        <v>7.8399999999999997E-3</v>
       </c>
       <c r="R3">
-        <v>0.19217400000000001</v>
+        <v>0.27885399999999999</v>
       </c>
       <c r="S3">
-        <v>0.21096799999999999</v>
+        <v>0.17976900000000001</v>
       </c>
       <c r="T3">
-        <v>6.3317999999999999E-2</v>
+        <v>6.2156999999999997E-2</v>
       </c>
       <c r="U3">
-        <v>5.8299999999999997E-4</v>
+        <v>1.1559999999999999E-3</v>
       </c>
       <c r="V3">
         <f t="shared" ref="V3:V9" si="7">SUM(R3:S3)</f>
-        <v>0.403142</v>
+        <v>0.458623</v>
       </c>
       <c r="W3">
         <f t="shared" si="2"/>
-        <v>0.46704299999999999</v>
+        <v>0.52193600000000007</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:23">
       <c r="A4" s="1">
         <v>1000</v>
       </c>
       <c r="B4">
-        <v>4.6100000000000002E-2</v>
+        <v>4.8899999999999999E-2</v>
       </c>
       <c r="C4">
-        <v>1.26E-2</v>
+        <v>1.06E-2</v>
       </c>
       <c r="D4">
         <v>1.34E-2</v>
       </c>
       <c r="E4">
         <f t="shared" si="3"/>
-        <v>5.8700000000000002E-2</v>
+        <v>5.9499999999999997E-2</v>
       </c>
       <c r="F4">
         <f t="shared" si="4"/>
-        <v>7.2099999999999997E-2</v>
+        <v>7.2899999999999993E-2</v>
       </c>
       <c r="G4">
-        <v>5.9400000000000001E-2</v>
+        <v>0.25729999999999997</v>
       </c>
       <c r="H4">
-        <v>0.31919999999999998</v>
+        <v>0.18840000000000001</v>
       </c>
       <c r="I4">
-        <v>6.1199999999999997E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="J4">
         <v>1.3599999999999999E-2</v>
       </c>
       <c r="K4">
         <f t="shared" si="5"/>
-        <v>0.37859999999999999</v>
+        <v>0.44569999999999999</v>
       </c>
       <c r="L4">
         <f t="shared" si="0"/>
-        <v>0.45339999999999997</v>
+        <v>0.52179999999999993</v>
       </c>
       <c r="M4">
-        <v>3.4388000000000002E-2</v>
+        <v>3.6158999999999997E-2</v>
       </c>
       <c r="N4">
-        <v>1.1872000000000001E-2</v>
+        <v>1.0755000000000001E-2</v>
       </c>
       <c r="O4">
-        <v>2.2729999999999998E-3</v>
+        <v>9.3439999999999999E-3</v>
       </c>
       <c r="P4">
         <f t="shared" si="6"/>
-        <v>4.6260000000000003E-2</v>
+        <v>4.6913999999999997E-2</v>
       </c>
       <c r="Q4">
         <f t="shared" si="1"/>
-        <v>4.8533E-2</v>
+        <v>5.6257999999999996E-2</v>
       </c>
       <c r="R4">
-        <v>0.186225</v>
+        <v>0.25766600000000001</v>
       </c>
       <c r="S4">
-        <v>0.24310399999999999</v>
+        <v>0.199818</v>
       </c>
       <c r="T4">
-        <v>6.6530000000000006E-2</v>
+        <v>6.1620000000000001E-2</v>
       </c>
       <c r="U4">
-        <v>4.7790000000000003E-3</v>
+        <v>9.4940000000000007E-3</v>
       </c>
       <c r="V4">
         <f t="shared" si="7"/>
-        <v>0.42932899999999996</v>
+        <v>0.457484</v>
       </c>
       <c r="W4">
         <f t="shared" si="2"/>
-        <v>0.50063799999999992</v>
+        <v>0.52859800000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:23">
       <c r="A5" s="1">
         <v>10000</v>
       </c>
       <c r="B5">
-        <v>0.43590000000000001</v>
+        <v>0.45610000000000001</v>
       </c>
       <c r="C5">
-        <v>0.1149</v>
+        <v>0.1163</v>
       </c>
       <c r="D5">
         <v>0.13370000000000001</v>
       </c>
       <c r="E5">
         <f t="shared" si="3"/>
-        <v>0.55079999999999996</v>
+        <v>0.57240000000000002</v>
       </c>
       <c r="F5">
         <f t="shared" si="4"/>
-        <v>0.6845</v>
+        <v>0.70610000000000006</v>
       </c>
       <c r="G5">
-        <v>5.79E-2</v>
+        <v>0.2717</v>
       </c>
       <c r="H5">
-        <v>0.3659</v>
+        <v>0.22520000000000001</v>
       </c>
       <c r="I5">
-        <v>9.6100000000000005E-2</v>
+        <v>8.6900000000000005E-2</v>
       </c>
       <c r="J5">
-        <v>0.1338</v>
+        <v>0.1348</v>
       </c>
       <c r="K5">
         <f t="shared" si="5"/>
-        <v>0.42380000000000001</v>
+        <v>0.49690000000000001</v>
       </c>
       <c r="L5">
         <f t="shared" si="0"/>
-        <v>0.65370000000000006</v>
+        <v>0.71860000000000002</v>
       </c>
       <c r="M5">
-        <v>0.331374</v>
+        <v>0.34958600000000001</v>
       </c>
       <c r="N5">
-        <v>0.12942100000000001</v>
+        <v>0.103018</v>
       </c>
       <c r="O5">
-        <v>2.4208E-2</v>
+        <v>9.3278E-2</v>
       </c>
       <c r="P5">
         <f t="shared" si="6"/>
-        <v>0.46079500000000001</v>
+        <v>0.45260400000000001</v>
       </c>
       <c r="Q5">
         <f t="shared" si="1"/>
-        <v>0.48500300000000002</v>
+        <v>0.54588199999999998</v>
       </c>
       <c r="R5">
-        <v>0.203847</v>
+        <v>0.26766800000000002</v>
       </c>
       <c r="S5">
-        <v>0.29677300000000001</v>
+        <v>0.23347300000000001</v>
       </c>
       <c r="T5">
-        <v>8.2985000000000003E-2</v>
+        <v>8.2072000000000006E-2</v>
       </c>
       <c r="U5">
-        <v>5.4524999999999997E-2</v>
+        <v>8.9680999999999997E-2</v>
       </c>
       <c r="V5">
         <f t="shared" si="7"/>
-        <v>0.50062000000000006</v>
+        <v>0.50114100000000006</v>
       </c>
       <c r="W5">
         <f t="shared" si="2"/>
-        <v>0.63813000000000009</v>
+        <v>0.6728940000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:23">
       <c r="A6" s="1">
         <v>100000</v>
       </c>
       <c r="B6">
-        <v>4.6462000000000003</v>
+        <v>4.7584</v>
       </c>
       <c r="C6">
-        <v>1.2143999999999999</v>
+        <v>1.3656999999999999</v>
       </c>
       <c r="D6">
-        <v>1.4245000000000001</v>
+        <v>1.3365</v>
       </c>
       <c r="E6">
         <f t="shared" si="3"/>
-        <v>5.8605999999999998</v>
+        <v>6.1241000000000003</v>
       </c>
       <c r="F6">
         <f t="shared" si="4"/>
-        <v>7.2850999999999999</v>
+        <v>7.4606000000000003</v>
       </c>
       <c r="G6">
-        <v>6.0600000000000001E-2</v>
+        <v>0.52939999999999998</v>
       </c>
       <c r="H6">
-        <v>1.2386999999999999</v>
+        <v>0.28749999999999998</v>
       </c>
       <c r="I6">
-        <v>0.51359999999999995</v>
+        <v>0.4889</v>
       </c>
       <c r="J6">
-        <v>1.3708</v>
+        <v>1.4012</v>
       </c>
       <c r="K6">
         <f t="shared" si="5"/>
-        <v>1.2992999999999999</v>
+        <v>0.81689999999999996</v>
       </c>
       <c r="L6">
         <f t="shared" si="0"/>
-        <v>3.1837</v>
+        <v>2.7069999999999999</v>
       </c>
       <c r="M6">
-        <v>3.3493400000000002</v>
+        <v>3.51335</v>
       </c>
       <c r="N6">
-        <v>1.3481300000000001</v>
+        <v>1.1242700000000001</v>
       </c>
       <c r="O6">
-        <v>0.23305300000000001</v>
+        <v>0.891127</v>
       </c>
       <c r="P6">
         <f t="shared" si="6"/>
-        <v>4.69747</v>
+        <v>4.6376200000000001</v>
       </c>
       <c r="Q6">
         <f t="shared" si="1"/>
-        <v>4.930523</v>
+        <v>5.5287470000000001</v>
       </c>
       <c r="R6">
-        <v>0.18995100000000001</v>
+        <v>0.61033300000000001</v>
       </c>
       <c r="S6">
-        <v>1.48854</v>
+        <v>0.35193799999999997</v>
       </c>
       <c r="T6">
-        <v>0.31885000000000002</v>
+        <v>0.52802099999999996</v>
       </c>
       <c r="U6">
-        <v>0.47934500000000002</v>
+        <v>0.90842299999999998</v>
       </c>
       <c r="V6">
         <f t="shared" si="7"/>
-        <v>1.678491</v>
+        <v>0.96227099999999999</v>
       </c>
       <c r="W6">
         <f t="shared" si="2"/>
-        <v>2.4766859999999999</v>
+        <v>2.3987150000000002</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:23">
       <c r="A7" s="1">
         <v>1000000</v>
       </c>
       <c r="B7">
-        <v>41.9816</v>
+        <v>42.9985</v>
       </c>
       <c r="C7">
-        <v>15.0382</v>
+        <v>14.2408</v>
       </c>
       <c r="D7">
-        <v>12.792</v>
+        <v>13.805400000000001</v>
       </c>
       <c r="E7">
         <f t="shared" si="3"/>
-        <v>57.019800000000004</v>
+        <v>57.2393</v>
       </c>
       <c r="F7">
         <f t="shared" si="4"/>
-        <v>69.811800000000005</v>
+        <v>71.044700000000006</v>
       </c>
       <c r="G7">
-        <v>0.17019999999999999</v>
+        <v>3.0855000000000001</v>
       </c>
       <c r="H7">
-        <v>5.6425000000000001</v>
+        <v>3.3714</v>
       </c>
       <c r="I7">
-        <v>4.1814999999999998</v>
+        <v>4.24</v>
       </c>
       <c r="J7">
-        <v>12.843299999999999</v>
+        <v>13.2249</v>
       </c>
       <c r="K7">
         <f t="shared" si="5"/>
-        <v>5.8127000000000004</v>
+        <v>6.4569000000000001</v>
       </c>
       <c r="L7">
         <f t="shared" si="0"/>
-        <v>22.837499999999999</v>
+        <v>23.921799999999998</v>
       </c>
       <c r="M7">
-        <v>31.771699999999999</v>
+        <v>34.297800000000002</v>
       </c>
       <c r="N7">
-        <v>15.199400000000001</v>
+        <v>11.5787</v>
       </c>
       <c r="O7">
-        <v>2.6561699999999999</v>
+        <v>8.4208700000000007</v>
       </c>
       <c r="P7">
         <f t="shared" si="6"/>
-        <v>46.9711</v>
+        <v>45.8765</v>
       </c>
       <c r="Q7">
         <f t="shared" si="1"/>
-        <v>49.627270000000003</v>
+        <v>54.297370000000001</v>
       </c>
       <c r="R7">
-        <v>0.40144400000000002</v>
+        <v>2.9301200000000001</v>
       </c>
       <c r="S7">
-        <v>5.6603300000000001</v>
+        <v>4.4267799999999999</v>
       </c>
       <c r="T7">
-        <v>5.20688</v>
+        <v>5.3120700000000003</v>
       </c>
       <c r="U7">
-        <v>4.4508200000000002</v>
+        <v>8.8368000000000002</v>
       </c>
       <c r="V7">
         <f t="shared" si="7"/>
-        <v>6.0617739999999998</v>
+        <v>7.3568999999999996</v>
       </c>
       <c r="W7">
         <f t="shared" si="2"/>
-        <v>15.719474</v>
+        <v>21.505769999999998</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:23">
       <c r="A8" s="1">
         <v>10000000</v>
       </c>
       <c r="B8">
-        <v>412.77499999999998</v>
+        <v>440.48099999999999</v>
       </c>
       <c r="C8">
-        <v>149.72</v>
+        <v>149.95500000000001</v>
       </c>
       <c r="D8">
-        <v>127.27500000000001</v>
+        <v>128.655</v>
       </c>
       <c r="E8">
         <f t="shared" si="3"/>
-        <v>562.495</v>
+        <v>590.43600000000004</v>
       </c>
       <c r="F8">
         <f t="shared" si="4"/>
-        <v>689.77</v>
+        <v>719.09100000000001</v>
       </c>
       <c r="G8">
-        <v>0.92459999999999998</v>
+        <v>25.2181</v>
       </c>
       <c r="H8">
-        <v>44.822099999999999</v>
+        <v>25.0867</v>
       </c>
       <c r="I8">
-        <v>39.967799999999997</v>
+        <v>43.5837</v>
       </c>
       <c r="J8">
-        <v>127.074</v>
+        <v>128.386</v>
       </c>
       <c r="K8">
         <f t="shared" si="5"/>
-        <v>45.746699999999997</v>
+        <v>50.3048</v>
       </c>
       <c r="L8">
         <f t="shared" si="0"/>
-        <v>212.7885</v>
+        <v>222.27449999999999</v>
       </c>
       <c r="M8">
-        <v>307.89400000000001</v>
+        <v>354.06599999999997</v>
       </c>
       <c r="N8">
-        <v>127.69</v>
+        <v>137.459</v>
       </c>
       <c r="O8">
-        <v>22.965199999999999</v>
+        <v>96.338300000000004</v>
       </c>
       <c r="P8">
         <f t="shared" si="6"/>
-        <v>435.584</v>
+        <v>491.52499999999998</v>
       </c>
       <c r="Q8">
         <f t="shared" si="1"/>
-        <v>458.54919999999998</v>
+        <v>587.86329999999998</v>
       </c>
       <c r="R8">
-        <v>1.5768500000000001</v>
+        <v>26.231300000000001</v>
       </c>
       <c r="S8">
-        <v>43.444499999999998</v>
+        <v>24.073499999999999</v>
       </c>
       <c r="T8">
-        <v>47.012700000000002</v>
+        <v>47.049199999999999</v>
       </c>
       <c r="U8">
-        <v>43.414999999999999</v>
+        <v>87.736099999999993</v>
       </c>
       <c r="V8">
         <f t="shared" si="7"/>
-        <v>45.021349999999998</v>
+        <v>50.3048</v>
       </c>
       <c r="W8">
         <f t="shared" si="2"/>
-        <v>135.44905</v>
+        <v>185.09010000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:23">
       <c r="A9" s="1">
         <v>100000000</v>
       </c>
       <c r="B9">
-        <v>4283.7299999999996</v>
+        <v>4538.3100000000004</v>
       </c>
       <c r="C9">
-        <v>1427.25</v>
+        <v>1573.75</v>
       </c>
       <c r="D9">
-        <v>1278.49</v>
+        <v>1301.3800000000001</v>
       </c>
       <c r="E9">
         <f t="shared" si="3"/>
-        <v>5710.98</v>
+        <v>6112.06</v>
       </c>
       <c r="F9">
         <f t="shared" si="4"/>
-        <v>6989.4699999999993</v>
+        <v>7413.4400000000005</v>
       </c>
       <c r="G9">
-        <v>2.8048999999999999</v>
+        <v>230.68799999999999</v>
       </c>
       <c r="H9">
-        <v>405.38400000000001</v>
+        <v>209.84</v>
       </c>
       <c r="I9">
-        <v>400.85500000000002</v>
+        <v>459.78500000000003</v>
       </c>
       <c r="J9">
-        <v>1301.2</v>
+        <v>1322.44</v>
       </c>
       <c r="K9">
         <f t="shared" si="5"/>
-        <v>408.18889999999999</v>
+        <v>440.52800000000002</v>
       </c>
       <c r="L9">
         <f t="shared" si="0"/>
-        <v>2110.2438999999999</v>
+        <v>2222.7530000000002</v>
       </c>
       <c r="M9">
-        <v>3130.81</v>
+        <v>3412.71</v>
       </c>
       <c r="N9">
-        <v>1366.69</v>
+        <v>1275.8900000000001</v>
       </c>
       <c r="O9">
-        <v>248.45500000000001</v>
+        <v>887.46199999999999</v>
       </c>
       <c r="P9">
         <f t="shared" si="6"/>
-        <v>4497.5</v>
+        <v>4688.6000000000004</v>
       </c>
       <c r="Q9">
         <f t="shared" si="1"/>
-        <v>4745.9549999999999</v>
+        <v>5576.0619999999999</v>
       </c>
       <c r="R9">
-        <v>7.3137499999999998</v>
+        <v>235.673</v>
       </c>
       <c r="S9">
-        <v>408.22899999999998</v>
+        <v>210.30600000000001</v>
       </c>
       <c r="T9">
-        <v>547.71600000000001</v>
+        <v>630.70399999999995</v>
       </c>
       <c r="U9">
-        <v>449.26600000000002</v>
+        <v>881.45399999999995</v>
       </c>
       <c r="V9">
         <f t="shared" si="7"/>
-        <v>415.54275000000001</v>
+        <v>445.97900000000004</v>
       </c>
       <c r="W9">
         <f t="shared" si="2"/>
-        <v>1412.52475</v>
+        <v>1958.1369999999999</v>
       </c>
     </row>
   </sheetData>
@@ -7916,36 +7911,36 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CF9CBA4-1D0E-4C7D-85A3-E5E8BE03303C}">
   <dimension ref="A1:W9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="1" width="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.1328125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.19921875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.53125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.53125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="17.796875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.19921875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="17.796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="17.9296875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.19921875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.19921875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="12.86328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="12.3984375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="12.53125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="17.59765625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="18.59765625" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.19921875" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.796875" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.9296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.8125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.5625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.8125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.1875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="17.8125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="17.9375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.1875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.1875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="12.375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12.5625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="18.625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.8125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.1875" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.8125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="18.9375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:23">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -8016,7 +8011,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:23">
       <c r="A2" s="1">
         <v>10</v>
       </c>
@@ -8095,7 +8090,7 @@
         <v>1.3681949999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:23">
       <c r="A3" s="1">
         <v>100</v>
       </c>
@@ -8174,7 +8169,7 @@
         <v>1.6355469999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:23">
       <c r="A4" s="1">
         <v>1000</v>
       </c>
@@ -8253,7 +8248,7 @@
         <v>1.7081529999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:23">
       <c r="A5" s="1">
         <v>10000</v>
       </c>
@@ -8332,7 +8327,7 @@
         <v>2.0617509999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:23">
       <c r="A6" s="1">
         <v>100000</v>
       </c>
@@ -8411,7 +8406,7 @@
         <v>4.7829629999999996</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:23">
       <c r="A7" s="1">
         <v>1000000</v>
       </c>
@@ -8490,7 +8485,7 @@
         <v>29.55997</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:23">
       <c r="A8" s="1">
         <v>10000000</v>
       </c>
@@ -8569,7 +8564,7 @@
         <v>252.88990000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:23">
       <c r="A9" s="1">
         <v>100000000</v>
       </c>

</xml_diff>